<commit_message>
astart program by command file
</commit_message>
<xml_diff>
--- a/config/data.xlsx
+++ b/config/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\python\sendTemplateMail\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5617382E-7F47-48E5-A5B6-B0A29822066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6ABFC4-B2E6-4BAB-A538-B0E615FD5348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>leave_date</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>D:\projects\python\sendTemplateMail\config\data.xlsx</t>
+  </si>
+  <si>
+    <t>cc_emails</t>
   </si>
 </sst>
 </file>
@@ -400,76 +403,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -477,8 +490,8 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F0C4FA34-364D-4082-9B9B-EF1FE1C1322F}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{88CFB4A1-67FB-42F1-B0DB-31DC096FB8D5}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{41AA2F49-2B73-4BBF-A6FA-50CF7651F3D1}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{03D5804E-01E7-4D41-9ACC-C2A00E3F7797}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{41AA2F49-2B73-4BBF-A6FA-50CF7651F3D1}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{03D5804E-01E7-4D41-9ACC-C2A00E3F7797}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
check attachment file mÃust be existed
</commit_message>
<xml_diff>
--- a/config/data.xlsx
+++ b/config/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\python\sendTemplateMail\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670550C4-9514-4F68-B290-A7021B13D7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEFF453-4A09-421A-9658-CBD57EB70240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>leave_date</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>D:\projects\python\sendTemplateMail\config\data.xlsx</t>
+  </si>
+  <si>
+    <t>cc_emails</t>
+  </si>
+  <si>
+    <t>D:\projects\python\sendTemplateMail\config_\data.xlsx</t>
   </si>
 </sst>
 </file>
@@ -400,80 +406,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -481,8 +493,8 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F0C4FA34-364D-4082-9B9B-EF1FE1C1322F}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{88CFB4A1-67FB-42F1-B0DB-31DC096FB8D5}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{41AA2F49-2B73-4BBF-A6FA-50CF7651F3D1}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{03D5804E-01E7-4D41-9ACC-C2A00E3F7797}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{41AA2F49-2B73-4BBF-A6FA-50CF7651F3D1}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{03D5804E-01E7-4D41-9ACC-C2A00E3F7797}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
fixed checking reminder_date is empty
</commit_message>
<xml_diff>
--- a/config/data.xlsx
+++ b/config/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\python\sendTemplateMail\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C1D20-4A84-43B1-B8DB-95E1F4947926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC13582-558D-479D-AC84-EC7C739D9E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>leave_date</t>
   </si>
@@ -54,9 +54,6 @@
     <t>full_name</t>
   </si>
   <si>
-    <t>nguyenminhhieu.geek@gmail.com</t>
-  </si>
-  <si>
     <t>bcc_emails</t>
   </si>
   <si>
@@ -72,16 +69,10 @@
     <t>17-09-2023</t>
   </si>
   <si>
-    <t>hieu.nguyenminh@chubb.com</t>
-  </si>
-  <si>
     <t>reminder_date</t>
   </si>
   <si>
     <t>2023-07-05 9:00</t>
-  </si>
-  <si>
-    <t>2023-07-05 14:00</t>
   </si>
   <si>
     <t>nmhillusion@hotmail.com</t>
@@ -418,7 +409,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,10 +429,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -456,17 +447,15 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
@@ -474,22 +463,20 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -498,20 +485,15 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F0C4FA34-364D-4082-9B9B-EF1FE1C1322F}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{41AA2F49-2B73-4BBF-A6FA-50CF7651F3D1}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{03D5804E-01E7-4D41-9ACC-C2A00E3F7797}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{BACBCE4C-2FFF-4072-A67D-AA45F27A4225}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{BACBCE4C-2FFF-4072-A67D-AA45F27A4225}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{58638E38-DD17-444A-9D94-E2B2BB26C678}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upgrade version dependencies for python 3.12
</commit_message>
<xml_diff>
--- a/config/data.xlsx
+++ b/config/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\python\sendTemplateMail\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\python\sendTemplateMail\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC13582-558D-479D-AC84-EC7C739D9E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11C6F78-E9C1-4FE5-99B9-3A48D621D237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>bcc_emails</t>
   </si>
   <si>
-    <t>D:\projects\python\sendTemplateMail\config\data.xlsx</t>
-  </si>
-  <si>
     <t>cc_emails</t>
   </si>
   <si>
@@ -75,7 +72,10 @@
     <t>2023-07-05 9:00</t>
   </si>
   <si>
-    <t>nmhillusion@hotmail.com</t>
+    <t>F:\python\sendTemplateMail\config\data.xlsx</t>
+  </si>
+  <si>
+    <t>nguyenminhhieu.geek@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -447,7 +447,7 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -463,10 +463,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -485,13 +485,13 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{BACBCE4C-2FFF-4072-A67D-AA45F27A4225}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{58638E38-DD17-444A-9D94-E2B2BB26C678}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{58638E38-DD17-444A-9D94-E2B2BB26C678}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{68FCF760-D9BE-47BB-9D79-34CAFF0EC1CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>